<commit_message>
fixed sequence id numbering and recomputed SASA for only charged substructures of basic residues
</commit_message>
<xml_diff>
--- a/Residue_ID_total_occupancy_10_1_2019.xlsx
+++ b/Residue_ID_total_occupancy_10_1_2019.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9982B2-EA68-9945-BD7D-C720587EB44B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6187C940-887C-C74C-9742-FDD538D4F232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="780" windowWidth="49220" windowHeight="26040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="780" windowWidth="20400" windowHeight="26040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cg" sheetId="2" r:id="rId1"/>
@@ -427,9 +427,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -447,6 +444,9 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -48319,26 +48319,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1DF7B5-858B-7A44-91C2-CCEE17B0F81A}">
   <dimension ref="A1:I1421"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -48372,7 +48372,7 @@
       <c r="H3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>71</v>
       </c>
     </row>
@@ -48531,23 +48531,23 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>793</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18">
         <v>12</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20">
+      <c r="E15" s="18"/>
+      <c r="F15" s="19">
         <v>1430</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19">
+      <c r="G15" s="18"/>
+      <c r="H15" s="18">
         <v>2848</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -49700,9 +49700,6 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>880</v>
-      </c>
       <c r="D98">
         <v>95</v>
       </c>
@@ -49747,6 +49744,9 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>880</v>
+      </c>
       <c r="D102">
         <v>99</v>
       </c>
@@ -53593,23 +53593,23 @@
       </c>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A378" s="21">
+      <c r="A378" s="20">
         <v>1156</v>
       </c>
-      <c r="B378" s="21"/>
-      <c r="C378" s="21"/>
-      <c r="D378" s="21">
+      <c r="B378" s="20"/>
+      <c r="C378" s="20"/>
+      <c r="D378" s="20">
         <v>375</v>
       </c>
-      <c r="E378" s="21"/>
-      <c r="F378" s="21">
+      <c r="E378" s="20"/>
+      <c r="F378" s="20">
         <v>1793</v>
       </c>
-      <c r="G378" s="21"/>
-      <c r="H378" s="22">
+      <c r="G378" s="20"/>
+      <c r="H378" s="21">
         <v>3211</v>
       </c>
-      <c r="I378" s="21"/>
+      <c r="I378" s="20"/>
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A379">
@@ -56748,23 +56748,23 @@
       </c>
     </row>
     <row r="603" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A603" s="21">
+      <c r="A603" s="20">
         <v>1508</v>
       </c>
-      <c r="B603" s="21"/>
-      <c r="C603" s="21"/>
-      <c r="D603" s="22">
+      <c r="B603" s="20"/>
+      <c r="C603" s="20"/>
+      <c r="D603" s="21">
         <v>600</v>
       </c>
-      <c r="E603" s="21"/>
-      <c r="F603" s="21">
+      <c r="E603" s="20"/>
+      <c r="F603" s="20">
         <v>2018</v>
       </c>
-      <c r="G603" s="21"/>
-      <c r="H603" s="21">
+      <c r="G603" s="20"/>
+      <c r="H603" s="20">
         <v>3436</v>
       </c>
-      <c r="I603" s="21" t="s">
+      <c r="I603" s="20" t="s">
         <v>73</v>
       </c>
     </row>
@@ -56858,7 +56858,7 @@
       </c>
       <c r="B610" s="15"/>
       <c r="C610" s="15"/>
-      <c r="D610" s="23">
+      <c r="D610" s="22">
         <v>607</v>
       </c>
       <c r="E610" s="15"/>
@@ -57565,7 +57565,7 @@
       </c>
       <c r="B660" s="15"/>
       <c r="C660" s="15"/>
-      <c r="D660" s="23">
+      <c r="D660" s="22">
         <v>657</v>
       </c>
       <c r="E660" s="15"/>
@@ -57586,7 +57586,7 @@
       </c>
       <c r="B661" s="15"/>
       <c r="C661" s="15"/>
-      <c r="D661" s="23">
+      <c r="D661" s="22">
         <v>658</v>
       </c>
       <c r="E661" s="15"/>
@@ -58036,23 +58036,23 @@
       </c>
     </row>
     <row r="693" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A693" s="19">
+      <c r="A693" s="18">
         <v>1674</v>
       </c>
-      <c r="B693" s="19"/>
-      <c r="C693" s="19"/>
-      <c r="D693" s="19">
+      <c r="B693" s="18"/>
+      <c r="C693" s="18"/>
+      <c r="D693" s="18">
         <v>690</v>
       </c>
-      <c r="E693" s="19"/>
-      <c r="F693" s="20">
+      <c r="E693" s="18"/>
+      <c r="F693" s="19">
         <v>2108</v>
       </c>
-      <c r="G693" s="19"/>
-      <c r="H693" s="19">
+      <c r="G693" s="18"/>
+      <c r="H693" s="18">
         <v>3526</v>
       </c>
-      <c r="I693" s="19" t="s">
+      <c r="I693" s="18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -58155,23 +58155,23 @@
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A701" s="24">
+      <c r="A701" s="23">
         <v>1682</v>
       </c>
-      <c r="B701" s="24"/>
-      <c r="C701" s="24"/>
-      <c r="D701" s="25">
+      <c r="B701" s="23"/>
+      <c r="C701" s="23"/>
+      <c r="D701" s="24">
         <v>698</v>
       </c>
-      <c r="E701" s="24"/>
-      <c r="F701" s="24">
+      <c r="E701" s="23"/>
+      <c r="F701" s="23">
         <v>2116</v>
       </c>
-      <c r="G701" s="24"/>
-      <c r="H701" s="24">
+      <c r="G701" s="23"/>
+      <c r="H701" s="23">
         <v>3534</v>
       </c>
-      <c r="I701" s="24" t="s">
+      <c r="I701" s="23" t="s">
         <v>75</v>
       </c>
     </row>
@@ -58218,23 +58218,23 @@
       </c>
     </row>
     <row r="705" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A705" s="24">
+      <c r="A705" s="23">
         <v>1686</v>
       </c>
-      <c r="B705" s="24"/>
-      <c r="C705" s="24"/>
-      <c r="D705" s="25">
+      <c r="B705" s="23"/>
+      <c r="C705" s="23"/>
+      <c r="D705" s="24">
         <v>702</v>
       </c>
-      <c r="E705" s="24"/>
-      <c r="F705" s="24">
+      <c r="E705" s="23"/>
+      <c r="F705" s="23">
         <v>2120</v>
       </c>
-      <c r="G705" s="24"/>
-      <c r="H705" s="24">
+      <c r="G705" s="23"/>
+      <c r="H705" s="23">
         <v>3538</v>
       </c>
-      <c r="I705" s="24" t="s">
+      <c r="I705" s="23" t="s">
         <v>75</v>
       </c>
     </row>
@@ -58673,23 +58673,23 @@
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A737" s="26">
+      <c r="A737" s="25">
         <v>1718</v>
       </c>
-      <c r="B737" s="26"/>
-      <c r="C737" s="26"/>
-      <c r="D737" s="26">
+      <c r="B737" s="25"/>
+      <c r="C737" s="25"/>
+      <c r="D737" s="25">
         <v>734</v>
       </c>
-      <c r="E737" s="26"/>
-      <c r="F737" s="26">
+      <c r="E737" s="25"/>
+      <c r="F737" s="25">
         <v>2152</v>
       </c>
-      <c r="G737" s="26"/>
-      <c r="H737" s="26">
+      <c r="G737" s="25"/>
+      <c r="H737" s="25">
         <v>3570</v>
       </c>
-      <c r="I737" s="26"/>
+      <c r="I737" s="25"/>
     </row>
     <row r="738" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A738">
@@ -60269,7 +60269,7 @@
         <v>847</v>
       </c>
       <c r="E850" s="12"/>
-      <c r="F850" s="27">
+      <c r="F850" s="26">
         <v>2265</v>
       </c>
       <c r="G850" s="12"/>
@@ -60290,7 +60290,7 @@
         <v>848</v>
       </c>
       <c r="E851" s="12"/>
-      <c r="F851" s="27">
+      <c r="F851" s="26">
         <v>2266</v>
       </c>
       <c r="G851" s="12"/>
@@ -60321,11 +60321,11 @@
       </c>
       <c r="B853" s="12"/>
       <c r="C853" s="12"/>
-      <c r="D853" s="27">
+      <c r="D853" s="26">
         <v>850</v>
       </c>
       <c r="E853" s="12"/>
-      <c r="F853" s="27">
+      <c r="F853" s="26">
         <v>2268</v>
       </c>
       <c r="G853" s="12"/>
@@ -62296,65 +62296,65 @@
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A999" s="28">
+      <c r="A999" s="27">
         <v>2124</v>
       </c>
-      <c r="B999" s="28"/>
-      <c r="C999" s="28"/>
-      <c r="D999" s="28">
+      <c r="B999" s="27"/>
+      <c r="C999" s="27"/>
+      <c r="D999" s="27">
         <v>996</v>
       </c>
-      <c r="E999" s="28"/>
-      <c r="F999" s="29">
+      <c r="E999" s="27"/>
+      <c r="F999" s="28">
         <v>2414</v>
       </c>
-      <c r="G999" s="28"/>
-      <c r="H999" s="28">
+      <c r="G999" s="27"/>
+      <c r="H999" s="27">
         <v>3832</v>
       </c>
-      <c r="I999" s="28" t="s">
+      <c r="I999" s="27" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="1000" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1000" s="28">
+      <c r="A1000" s="27">
         <v>2125</v>
       </c>
-      <c r="B1000" s="28"/>
-      <c r="C1000" s="28"/>
-      <c r="D1000" s="28">
+      <c r="B1000" s="27"/>
+      <c r="C1000" s="27"/>
+      <c r="D1000" s="27">
         <v>997</v>
       </c>
-      <c r="E1000" s="28"/>
-      <c r="F1000" s="29">
+      <c r="E1000" s="27"/>
+      <c r="F1000" s="28">
         <v>2415</v>
       </c>
-      <c r="G1000" s="28"/>
-      <c r="H1000" s="28">
+      <c r="G1000" s="27"/>
+      <c r="H1000" s="27">
         <v>3833</v>
       </c>
-      <c r="I1000" s="28" t="s">
+      <c r="I1000" s="27" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="1001" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1001" s="28">
+      <c r="A1001" s="27">
         <v>2126</v>
       </c>
-      <c r="B1001" s="28"/>
-      <c r="C1001" s="28"/>
-      <c r="D1001" s="28">
+      <c r="B1001" s="27"/>
+      <c r="C1001" s="27"/>
+      <c r="D1001" s="27">
         <v>998</v>
       </c>
-      <c r="E1001" s="28"/>
-      <c r="F1001" s="29">
+      <c r="E1001" s="27"/>
+      <c r="F1001" s="28">
         <v>2416</v>
       </c>
-      <c r="G1001" s="28"/>
-      <c r="H1001" s="28">
+      <c r="G1001" s="27"/>
+      <c r="H1001" s="27">
         <v>3834</v>
       </c>
-      <c r="I1001" s="28" t="s">
+      <c r="I1001" s="27" t="s">
         <v>78</v>
       </c>
     </row>
@@ -62632,44 +62632,44 @@
       </c>
     </row>
     <row r="1021" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1021" s="21">
+      <c r="A1021" s="20">
         <v>2146</v>
       </c>
-      <c r="B1021" s="21"/>
-      <c r="C1021" s="21"/>
-      <c r="D1021" s="21">
+      <c r="B1021" s="20"/>
+      <c r="C1021" s="20"/>
+      <c r="D1021" s="20">
         <v>1018</v>
       </c>
-      <c r="E1021" s="21"/>
-      <c r="F1021" s="21">
+      <c r="E1021" s="20"/>
+      <c r="F1021" s="20">
         <v>2436</v>
       </c>
-      <c r="G1021" s="21"/>
-      <c r="H1021" s="21">
+      <c r="G1021" s="20"/>
+      <c r="H1021" s="20">
         <v>3854</v>
       </c>
-      <c r="I1021" s="21" t="s">
+      <c r="I1021" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="1022" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1022" s="21">
+      <c r="A1022" s="20">
         <v>2147</v>
       </c>
-      <c r="B1022" s="21"/>
-      <c r="C1022" s="21"/>
-      <c r="D1022" s="21">
+      <c r="B1022" s="20"/>
+      <c r="C1022" s="20"/>
+      <c r="D1022" s="20">
         <v>1019</v>
       </c>
-      <c r="E1022" s="21"/>
-      <c r="F1022" s="21">
+      <c r="E1022" s="20"/>
+      <c r="F1022" s="20">
         <v>2437</v>
       </c>
-      <c r="G1022" s="21"/>
-      <c r="H1022" s="21">
+      <c r="G1022" s="20"/>
+      <c r="H1022" s="20">
         <v>3855</v>
       </c>
-      <c r="I1022" s="21" t="s">
+      <c r="I1022" s="20" t="s">
         <v>73</v>
       </c>
     </row>
@@ -63178,23 +63178,23 @@
       </c>
     </row>
     <row r="1059" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1059" s="21">
+      <c r="A1059" s="20">
         <v>2184</v>
       </c>
-      <c r="B1059" s="21"/>
-      <c r="C1059" s="21"/>
-      <c r="D1059" s="21">
+      <c r="B1059" s="20"/>
+      <c r="C1059" s="20"/>
+      <c r="D1059" s="20">
         <v>1056</v>
       </c>
-      <c r="E1059" s="21"/>
-      <c r="F1059" s="21">
+      <c r="E1059" s="20"/>
+      <c r="F1059" s="20">
         <v>2474</v>
       </c>
-      <c r="G1059" s="21"/>
-      <c r="H1059" s="21">
+      <c r="G1059" s="20"/>
+      <c r="H1059" s="20">
         <v>3892</v>
       </c>
-      <c r="I1059" s="21" t="s">
+      <c r="I1059" s="20" t="s">
         <v>73</v>
       </c>
     </row>
@@ -63332,23 +63332,23 @@
       </c>
     </row>
     <row r="1069" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1069" s="30">
+      <c r="A1069" s="29">
         <v>2194</v>
       </c>
-      <c r="B1069" s="30"/>
-      <c r="C1069" s="30"/>
-      <c r="D1069" s="31">
+      <c r="B1069" s="29"/>
+      <c r="C1069" s="29"/>
+      <c r="D1069" s="30">
         <v>1066</v>
       </c>
-      <c r="E1069" s="30"/>
-      <c r="F1069" s="30">
+      <c r="E1069" s="29"/>
+      <c r="F1069" s="29">
         <v>2484</v>
       </c>
-      <c r="G1069" s="30"/>
-      <c r="H1069" s="30">
+      <c r="G1069" s="29"/>
+      <c r="H1069" s="29">
         <v>3902</v>
       </c>
-      <c r="I1069" s="30" t="s">
+      <c r="I1069" s="29" t="s">
         <v>79</v>
       </c>
     </row>
@@ -63591,23 +63591,23 @@
       </c>
     </row>
     <row r="1087" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1087" s="32">
+      <c r="A1087" s="31">
         <v>2212</v>
       </c>
-      <c r="B1087" s="32"/>
-      <c r="C1087" s="32"/>
-      <c r="D1087" s="32">
+      <c r="B1087" s="31"/>
+      <c r="C1087" s="31"/>
+      <c r="D1087" s="31">
         <v>1084</v>
       </c>
-      <c r="E1087" s="32"/>
-      <c r="F1087" s="33">
+      <c r="E1087" s="31"/>
+      <c r="F1087" s="32">
         <v>2502</v>
       </c>
-      <c r="G1087" s="32"/>
-      <c r="H1087" s="32">
+      <c r="G1087" s="31"/>
+      <c r="H1087" s="31">
         <v>3920</v>
       </c>
-      <c r="I1087" s="32" t="s">
+      <c r="I1087" s="31" t="s">
         <v>80</v>
       </c>
     </row>
@@ -66992,21 +66992,21 @@
       </c>
     </row>
     <row r="1332" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1332" s="32"/>
-      <c r="B1332" s="32"/>
-      <c r="C1332" s="32"/>
-      <c r="D1332" s="32">
+      <c r="A1332" s="31"/>
+      <c r="B1332" s="31"/>
+      <c r="C1332" s="31"/>
+      <c r="D1332" s="31">
         <v>1329</v>
       </c>
-      <c r="E1332" s="32"/>
-      <c r="F1332" s="33">
+      <c r="E1332" s="31"/>
+      <c r="F1332" s="32">
         <v>2747</v>
       </c>
-      <c r="G1332" s="32"/>
-      <c r="H1332" s="32">
+      <c r="G1332" s="31"/>
+      <c r="H1332" s="31">
         <v>4165</v>
       </c>
-      <c r="I1332" s="32" t="s">
+      <c r="I1332" s="31" t="s">
         <v>80</v>
       </c>
     </row>
@@ -67022,21 +67022,21 @@
       </c>
     </row>
     <row r="1334" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1334" s="32"/>
-      <c r="B1334" s="32"/>
-      <c r="C1334" s="32"/>
-      <c r="D1334" s="32">
+      <c r="A1334" s="31"/>
+      <c r="B1334" s="31"/>
+      <c r="C1334" s="31"/>
+      <c r="D1334" s="31">
         <v>1331</v>
       </c>
-      <c r="E1334" s="32"/>
-      <c r="F1334" s="33">
+      <c r="E1334" s="31"/>
+      <c r="F1334" s="32">
         <v>2749</v>
       </c>
-      <c r="G1334" s="32"/>
-      <c r="H1334" s="32">
+      <c r="G1334" s="31"/>
+      <c r="H1334" s="31">
         <v>4167</v>
       </c>
-      <c r="I1334" s="32" t="s">
+      <c r="I1334" s="31" t="s">
         <v>80</v>
       </c>
     </row>
@@ -67102,23 +67102,23 @@
       </c>
     </row>
     <row r="1340" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1340" s="32">
+      <c r="A1340" s="31">
         <v>2465</v>
       </c>
-      <c r="B1340" s="32"/>
-      <c r="C1340" s="32"/>
-      <c r="D1340" s="32">
+      <c r="B1340" s="31"/>
+      <c r="C1340" s="31"/>
+      <c r="D1340" s="31">
         <v>1337</v>
       </c>
-      <c r="E1340" s="32"/>
-      <c r="F1340" s="33">
+      <c r="E1340" s="31"/>
+      <c r="F1340" s="32">
         <v>2755</v>
       </c>
-      <c r="G1340" s="32"/>
-      <c r="H1340" s="32">
+      <c r="G1340" s="31"/>
+      <c r="H1340" s="31">
         <v>4173</v>
       </c>
-      <c r="I1340" s="32" t="s">
+      <c r="I1340" s="31" t="s">
         <v>80</v>
       </c>
     </row>
@@ -67361,23 +67361,23 @@
       </c>
     </row>
     <row r="1358" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1358" s="28">
+      <c r="A1358" s="27">
         <v>2483</v>
       </c>
-      <c r="B1358" s="28"/>
-      <c r="C1358" s="28"/>
-      <c r="D1358" s="28">
+      <c r="B1358" s="27"/>
+      <c r="C1358" s="27"/>
+      <c r="D1358" s="27">
         <v>1355</v>
       </c>
-      <c r="E1358" s="28"/>
-      <c r="F1358" s="29">
+      <c r="E1358" s="27"/>
+      <c r="F1358" s="28">
         <v>2773</v>
       </c>
-      <c r="G1358" s="28"/>
-      <c r="H1358" s="28">
+      <c r="G1358" s="27"/>
+      <c r="H1358" s="27">
         <v>4191</v>
       </c>
-      <c r="I1358" s="28" t="s">
+      <c r="I1358" s="27" t="s">
         <v>78</v>
       </c>
     </row>
@@ -67396,23 +67396,23 @@
       </c>
     </row>
     <row r="1360" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1360" s="30">
+      <c r="A1360" s="29">
         <v>2485</v>
       </c>
-      <c r="B1360" s="30"/>
-      <c r="C1360" s="30"/>
-      <c r="D1360" s="31">
+      <c r="B1360" s="29"/>
+      <c r="C1360" s="29"/>
+      <c r="D1360" s="30">
         <v>1357</v>
       </c>
-      <c r="E1360" s="30"/>
-      <c r="F1360" s="30">
+      <c r="E1360" s="29"/>
+      <c r="F1360" s="29">
         <v>2775</v>
       </c>
-      <c r="G1360" s="30"/>
-      <c r="H1360" s="30">
+      <c r="G1360" s="29"/>
+      <c r="H1360" s="29">
         <v>4193</v>
       </c>
-      <c r="I1360" s="30" t="s">
+      <c r="I1360" s="29" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>